<commit_message>
added type script and java script languages function extraction
</commit_message>
<xml_diff>
--- a/test_resource/codeextractor_T_T_A.xlsx
+++ b/test_resource/codeextractor_T_T_A.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="183">
   <si>
     <t>Code</t>
   </si>
@@ -22,265 +22,277 @@
     <t>Uniq ID</t>
   </si>
   <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_afterAll</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_beforeAll</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_getCerberusCommandLineUsageString</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCallMethod</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebrusWithArguments</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebruswithOutArguments</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebruswithWrongArguments</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\HelloController.java_index1</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\HelloController.java_index2</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\HelloController.java_meth</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\python_annot_file.py_create_parser</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\python_annot_file.py_validate_return</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\python_file.py_create_parser</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_c.c_main</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_c.c_swap</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_cpp_code.cpp_main</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_cpp_code.cpp_relational_operation</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_generate_pylint_cmd</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_check_pass_fail_status</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_file_name</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_guardrails_obj</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_log_data</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_test_guardrail_gate_status</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_test_guardrail_gate_status_fail</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_validate_return</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_return_jscpd_false</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_setUp</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_stub_get_all_func_cnn</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_stub_globals</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_stub_validate_return</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_tearDown</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_call_subprocess_error</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_call_subprocess_noerror</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_check_pass_fail_success</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_check_report_dir</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_file_exists</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_file_exists_exit</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_get_all_func_cnn</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_get_index_cnn</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_coverage</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_coverage_fail</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_cyclomatic_complexity</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_deadcode</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_deadcode_fail</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_jscpd</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_jscpd_fail</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_lint</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_mutation</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_test</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_test_fail</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_list_to_str_folders</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_mov_cov_report</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_orchestrate_guardrails</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_parse_cyclo_report_xml</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_parse_jscpd_report_json</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_parse_mutmut_report_xml</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_validate_return</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_ARSorting</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_AutoRefreshImport</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_ChangePatientDetails</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_Choosefolder</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_DeidentifyPatientDetails</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_DeleteAllStudies</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_GetPictorialIndex</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_GetPictorialIndexSeriesNobyDescription</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_PIContextMenuCopyTo</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_PIContextMenuCopyToRighClick</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_PIToggle</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_ProgressBar</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_RightClickPISelectedSeries</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_RunScriptsinRemoteSystem</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_SelectPISeriesByMouseHover</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_SelectPictorialSeriesByIndexvalue</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_SelectPictorialSeriesBySeriesValue</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_SeriesFilesCount</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_SeriesReportCount</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_SeriesSelect</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_VerifyCSROIApplication</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_VerifyisPatientSelected</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_runNetworkLogin</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\src\test_repo.java_runNetworkLogout</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\test\TestHelloController.java_Test_AddMethod</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\tst\TstHelloController.java_Test_AddMethod</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_AddMethod</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_DivideMethod</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_MultiplyMethod</t>
-  </si>
-  <si>
-    <t>C:\Users\320074769\Downloads\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_SubstractMethod</t>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_afterAll</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_beforeAll</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_getCerberusCommandLineUsageString</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCallMethod</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebrusWithArguments</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebruswithOutArguments</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\CerberusTest.java_testCerebruswithWrongArguments</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\HelloController.java_index1</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\HelloController.java_index2</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\HelloController.java_meth</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\python_annot_file.py_create_parser</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\python_annot_file.py_validate_return</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\python_file.py_create_parser</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_c.c_main</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_c.c_swap</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_cpp_code.cpp_main</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_cpp_code.cpp_relational_operation</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_generate_pylint_cmd</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_check_pass_fail_status</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_file_name</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_guardrails_obj</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_log_data</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_test_guardrail_gate_status</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_test_guardrail_gate_status_fail</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_get_validate_return</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_return_jscpd_false</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_setUp</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_stub_get_all_func_cnn</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_stub_globals</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_stub_validate_return</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_tearDown</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_call_subprocess_error</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_call_subprocess_noerror</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_check_pass_fail_success</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_check_report_dir</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_file_exists</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_file_exists_exit</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_get_all_func_cnn</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_get_index_cnn</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_coverage</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_coverage_fail</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_cyclomatic_complexity</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_deadcode</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_deadcode_fail</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_jscpd</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_jscpd_fail</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_lint</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_mutation</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_test</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_guardrail_test_fail</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_list_to_str_folders</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_mov_cov_report</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_orchestrate_guardrails</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_parse_cyclo_report_xml</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_parse_jscpd_report_json</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_parse_mutmut_report_xml</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_guardrails.py_test_validate_return</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_ARSorting</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_AutoRefreshImport</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_ChangePatientDetails</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_Choosefolder</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_DeidentifyPatientDetails</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_DeleteAllStudies</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_GetPictorialIndex</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_GetPictorialIndexSeriesNobyDescription</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_PIContextMenuCopyTo</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_PIContextMenuCopyToRighClick</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_PIToggle</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_ProgressBar</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_RightClickPISelectedSeries</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_RunScriptsinRemoteSystem</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_SelectPISeriesByMouseHover</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_SelectPictorialSeriesByIndexvalue</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_SelectPictorialSeriesBySeriesValue</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_SeriesFilesCount</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_SeriesReportCount</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_SeriesSelect</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_VerifyCSROIApplication</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_VerifyisPatientSelected</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_runNetworkLogin</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\test_repo.java_runNetworkLogout</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\typescript_sample.js_Student</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\typescript_sample.js_greeter</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\typescript_sample.ts_constructor</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\src\typescript_sample.ts_greeter</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\test\TestHelloController.java_Test_AddMethod</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\tst\TstHelloController.java_Test_AddMethod</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_AddMethod</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_DivideMethod</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_MultiplyMethod</t>
+  </si>
+  <si>
+    <t>C:\Users\320074769\Downloads\Python_Repos\funcSSH\functiondefextractor\test_resource\test_repo\tst\test.cs_Test_SubstractMethod</t>
   </si>
   <si>
     <t xml:space="preserve">public void afterAll() {_x000D_
@@ -1988,6 +2000,36 @@
 Tasks = NetworkSuite["Jobs"]["ItemByName"]("Login")["Tasks"]_x000D_
 Task = Tasks["Items"](2)_x000D_
 Task["Run"](true)_x000D_
+}_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var Student = /** @class */ (function () {_x000D_
+function Student(firstName, middleInitial, lastName) {_x000D_
+this.firstName = firstName_x000D_
+this.middleInitial = middleInitial_x000D_
+this.lastName = lastName_x000D_
+this.fullName = firstName + " " + middleInitial + " " + lastName_x000D_
+}_x000D_
+return Student_x000D_
+}())_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function greeter(person) {_x000D_
+return "Hello, " + person.firstName + " " + person.lastName_x000D_
+}_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constructor(public firstName: string, public middleInitial: string, public lastName: string) {_x000D_
+this.fullName = firstName + " " + middleInitial + " " + lastName_x000D_
+}_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function greeter(person: Person) {_x000D_
+return "Hello, " + person.firstName + " " + person.lastName_x000D_
 }_x000D_
 </t>
   </si>
@@ -2395,7 +2437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2414,7 +2456,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2422,7 +2464,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2430,7 +2472,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2438,7 +2480,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2446,7 +2488,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2454,7 +2496,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2462,7 +2504,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2470,7 +2512,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2478,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2486,7 +2528,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2494,7 +2536,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2502,7 +2544,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2510,7 +2552,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2518,7 +2560,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2526,7 +2568,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2534,7 +2576,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2542,7 +2584,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2550,7 +2592,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2558,7 +2600,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2566,7 +2608,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2574,7 +2616,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2582,7 +2624,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2590,7 +2632,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2598,7 +2640,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2606,7 +2648,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2614,7 +2656,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2622,7 +2664,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -2630,7 +2672,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2638,7 +2680,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2646,7 +2688,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2654,7 +2696,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2662,7 +2704,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2670,7 +2712,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2678,7 +2720,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2686,7 +2728,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2694,7 +2736,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2702,7 +2744,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -2710,7 +2752,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -2718,7 +2760,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -2726,7 +2768,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2734,7 +2776,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2742,7 +2784,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2750,7 +2792,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2758,7 +2800,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2766,7 +2808,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2774,7 +2816,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2782,7 +2824,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2790,7 +2832,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2798,7 +2840,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2806,7 +2848,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2814,7 +2856,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2822,7 +2864,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2830,7 +2872,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2838,7 +2880,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2846,7 +2888,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2854,7 +2896,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2862,7 +2904,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2870,7 +2912,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2878,7 +2920,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2886,7 +2928,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2894,7 +2936,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2902,7 +2944,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2910,7 +2952,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2918,7 +2960,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2926,7 +2968,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2934,7 +2976,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2942,7 +2984,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2950,7 +2992,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2958,7 +3000,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2966,7 +3008,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2974,7 +3016,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2982,7 +3024,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2990,7 +3032,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2998,7 +3040,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -3006,7 +3048,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -3014,7 +3056,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -3022,7 +3064,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -3030,7 +3072,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -3038,7 +3080,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3046,7 +3088,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3054,7 +3096,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3062,55 +3104,55 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3118,7 +3160,39 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>174</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>